<commit_message>
incremental dataset updates halfway done
</commit_message>
<xml_diff>
--- a/configurations/experiment_configs.xlsx
+++ b/configurations/experiment_configs.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="188">
   <si>
     <t xml:space="preserve">var_name</t>
   </si>
@@ -580,6 +580,15 @@
   </si>
   <si>
     <t xml:space="preserve">192</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uls23_bone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sourcepatch</t>
   </si>
 </sst>
 </file>
@@ -886,7 +895,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4:S4"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1219,7 +1228,7 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="1" sqref="E4:S4 A13"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1440,7 +1449,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L48" activeCellId="1" sqref="E4:S4 L48"/>
+      <selection pane="topLeft" activeCell="L48" activeCellId="0" sqref="L48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1681,7 +1690,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="E4:S4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1804,7 +1813,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="E4:S4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1894,10 +1903,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AE27"/>
+  <dimension ref="A1:AE28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S4" activeCellId="0" sqref="E4:S4"/>
+      <selection pane="topLeft" activeCell="I29" activeCellId="0" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2831,7 +2840,6 @@
       <c r="O23" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="Q23" s="0"/>
       <c r="S23" s="1" t="s">
         <v>160</v>
       </c>
@@ -3006,6 +3014,45 @@
       </c>
       <c r="AE27" s="1" t="n">
         <v>10</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B28" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="R28" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T28" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="U28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V28" s="4" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="Y28" s="1" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
critical bugs fixed in imported data analyser
</commit_message>
<xml_diff>
--- a/configurations/experiment_configs.xlsx
+++ b/configurations/experiment_configs.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="188">
   <si>
     <t xml:space="preserve">var_name</t>
   </si>
@@ -552,7 +552,7 @@
     <t xml:space="preserve">lidc</t>
   </si>
   <si>
-    <t xml:space="preserve">$cold_storage_folder/predictions/totalseg/LITS-1271</t>
+    <t xml:space="preserve">$cold_storage_folder/predictions/totalseg/LITS-1439</t>
   </si>
   <si>
     <t xml:space="preserve">TSL.label_localiser,TSL.lungs</t>
@@ -679,24 +679,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -905,7 +901,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="1" width="20.09"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -937,275 +933,275 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3" t="n">
+      <c r="D3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="n">
         <v>0.001</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="D5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="J5" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="D6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="D7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="D8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="D9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="D10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="D11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" s="3" t="s">
+      <c r="D12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" s="3" t="s">
+      <c r="D13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" s="3" t="s">
+      <c r="D14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" s="3" t="s">
+      <c r="D15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E16" s="3" t="s">
+      <c r="D16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E17" s="3" t="s">
+      <c r="D17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1236,7 +1232,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="24.78"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1271,165 +1267,162 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="K6" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="D7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="D8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="D9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="1" t="s">
         <v>78</v>
       </c>
       <c r="E10" s="1" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3"/>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
         <v>80</v>
       </c>
       <c r="E14" s="1" t="n">
         <v>192</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
         <v>81</v>
       </c>
       <c r="E15" s="1" t="n">
         <v>128</v>
       </c>
     </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1458,7 +1451,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.38"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1484,190 +1477,190 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F2" s="3" t="n">
+      <c r="F2" s="1" t="n">
         <v>0.1</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="3" t="n">
+      <c r="F3" s="1" t="n">
         <v>0.1</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="1" t="n">
         <v>0.1</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F5" s="3" t="n">
+      <c r="F5" s="1" t="n">
         <v>0.1</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="B6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F6" s="3" t="n">
+      <c r="F6" s="1" t="n">
         <v>0.1</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="F7" s="3" t="n">
+      <c r="F7" s="1" t="n">
         <v>0.1</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B8" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="B8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F8" s="3" t="n">
+      <c r="F8" s="1" t="n">
         <v>0.1</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="B9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="3" t="n">
+      <c r="F9" s="1" t="n">
         <v>0.1</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1695,7 +1688,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1715,82 +1708,82 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="D5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="D6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1818,7 +1811,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1838,52 +1831,52 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D2" s="3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="D2" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="D5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="D5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="D6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1906,7 +1899,7 @@
   <dimension ref="A1:AE28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I29" activeCellId="0" sqref="I29"/>
+      <selection pane="topLeft" activeCell="O35" activeCellId="0" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1926,7 +1919,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="23" style="1" width="8.59"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>125</v>
       </c>
@@ -2021,7 +2014,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>149</v>
       </c>
@@ -2055,12 +2048,12 @@
       <c r="U2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="4" t="b">
+      <c r="V2" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>149</v>
       </c>
@@ -2103,12 +2096,12 @@
       <c r="U3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="V3" s="4" t="b">
+      <c r="V3" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>149</v>
       </c>
@@ -2145,12 +2138,12 @@
       <c r="U4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="V4" s="4" t="b">
+      <c r="V4" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>149</v>
       </c>
@@ -2181,12 +2174,12 @@
       <c r="U5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="V5" s="4" t="b">
+      <c r="V5" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>149</v>
       </c>
@@ -2220,12 +2213,12 @@
       <c r="U6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="V6" s="4" t="b">
+      <c r="V6" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>149</v>
       </c>
@@ -2265,12 +2258,12 @@
       <c r="U7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="V7" s="4" t="b">
+      <c r="V7" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>149</v>
       </c>
@@ -2310,12 +2303,12 @@
       <c r="U8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="V8" s="4" t="b">
+      <c r="V8" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>149</v>
       </c>
@@ -2355,12 +2348,12 @@
       <c r="U9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="V9" s="4" t="b">
+      <c r="V9" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>161</v>
       </c>
@@ -2391,12 +2384,12 @@
       <c r="T10" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="V10" s="4" t="b">
+      <c r="V10" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>161</v>
       </c>
@@ -2421,12 +2414,12 @@
       <c r="T11" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="V11" s="4" t="b">
+      <c r="V11" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>161</v>
       </c>
@@ -2454,12 +2447,12 @@
       <c r="T12" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="V12" s="4" t="b">
+      <c r="V12" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>161</v>
       </c>
@@ -2484,12 +2477,12 @@
       <c r="T13" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="V13" s="4" t="b">
+      <c r="V13" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>161</v>
       </c>
@@ -2517,7 +2510,7 @@
       <c r="T14" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="V14" s="4" t="b">
+      <c r="V14" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2525,7 +2518,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>161</v>
       </c>
@@ -2553,12 +2546,12 @@
       <c r="T15" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="V15" s="4" t="b">
+      <c r="V15" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>161</v>
       </c>
@@ -2577,12 +2570,12 @@
       <c r="S16" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="V16" s="4" t="b">
+      <c r="V16" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>161</v>
       </c>
@@ -2610,12 +2603,12 @@
       <c r="T17" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="V17" s="4" t="b">
+      <c r="V17" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>161</v>
       </c>
@@ -2646,12 +2639,12 @@
       <c r="T18" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="V18" s="4" t="b">
+      <c r="V18" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>161</v>
       </c>
@@ -2676,12 +2669,12 @@
       <c r="T19" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="V19" s="4" t="b">
+      <c r="V19" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>173</v>
       </c>
@@ -2697,7 +2690,7 @@
       <c r="F20" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="H20" s="4" t="b">
+      <c r="H20" s="3" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2725,12 +2718,12 @@
       <c r="U20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="V20" s="4" t="b">
+      <c r="V20" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>173</v>
       </c>
@@ -2740,13 +2733,13 @@
       <c r="C21" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>34</v>
+      <c r="D21" s="1" t="n">
+        <v>50</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="H21" s="4" t="b">
+      <c r="H21" s="3" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2774,12 +2767,12 @@
       <c r="U21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="V21" s="4" t="b">
+      <c r="V21" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>177</v>
       </c>
@@ -2807,7 +2800,7 @@
       <c r="U22" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="V22" s="4" t="b">
+      <c r="V22" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2815,7 +2808,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>177</v>
       </c>
@@ -2846,7 +2839,7 @@
       <c r="U23" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="V23" s="4" t="b">
+      <c r="V23" s="3" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -2854,7 +2847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>177</v>
       </c>
@@ -2885,7 +2878,7 @@
       <c r="U24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="V24" s="4" t="b">
+      <c r="V24" s="3" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2893,7 +2886,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>177</v>
       </c>
@@ -2924,7 +2917,7 @@
       <c r="U25" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="V25" s="4" t="b">
+      <c r="V25" s="3" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2932,7 +2925,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>177</v>
       </c>
@@ -2966,7 +2959,7 @@
       <c r="U26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="V26" s="4" t="b">
+      <c r="V26" s="3" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2974,7 +2967,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>177</v>
       </c>
@@ -3008,7 +3001,7 @@
       <c r="U27" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="V27" s="4" t="b">
+      <c r="V27" s="3" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -3016,7 +3009,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>185</v>
       </c>
@@ -3047,7 +3040,7 @@
       <c r="U28" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="V28" s="4" t="b">
+      <c r="V28" s="3" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>

</xml_diff>